<commit_message>
MPESIMO 10082025 0658PM UPDATED
</commit_message>
<xml_diff>
--- a/Portal/AttendanceCorrectionAttachments/Attendance_Correction_Template.xlsx
+++ b/Portal/AttendanceCorrectionAttachments/Attendance_Correction_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APW System\APWPortal-Web-UI\Portal\AttendanceCorrectionAttachments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APW SYSTEM\SOURCE CODE\APWPortal-WEB-UI\Portal\AttendanceCorrectionAttachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F4E464-B566-4A84-84CF-3BB51F542B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EED18C-02E2-46B8-92B7-472449EC1645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{8BE08107-396F-4978-B693-58822A82BF65}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8BE08107-396F-4978-B693-58822A82BF65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -259,11 +259,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -272,36 +352,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -315,9 +370,6 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -330,9 +382,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -345,9 +394,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -355,6 +408,38 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -362,6 +447,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AED674C-8533-4677-952F-64DCC057D066}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection sqref="A1:J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,504 +859,536 @@
     <col min="7" max="7" width="3.85546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="11.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="3.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="8" style="2" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-    </row>
-    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-    </row>
-    <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="I3" s="5"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-    </row>
-    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="I4" s="5"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-    </row>
-    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-    </row>
-    <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="C6" s="13" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="26"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="26"/>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="G8" s="7" t="s">
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="26"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="26"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="C10" s="7" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="26"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="C11" s="7" t="s">
+      <c r="D10" s="29"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-    </row>
-    <row r="13" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="C13" s="8" t="s">
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="C14" s="7" t="s">
+      <c r="D13" s="31"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="26"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="C15" s="7" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-    </row>
-    <row r="17" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="C17" s="8" t="s">
+      <c r="D15" s="29"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="26"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="26"/>
+    </row>
+    <row r="17" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="22"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="25"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="25"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="28"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="C23" s="3" t="s">
+      <c r="D17" s="23"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="26"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="26"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="26"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="26"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="D23" s="24"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="C26" s="12" t="s">
+      <c r="I23" s="23"/>
+      <c r="J23" s="26"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="26"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="26"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="12" t="s">
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I26" s="12"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="C28" s="3" t="s">
+      <c r="I26" s="35"/>
+      <c r="J26" s="26"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="26"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="22"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="D28" s="24"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="C31" s="12" t="s">
+      <c r="I28" s="23"/>
+      <c r="J28" s="26"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="26"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="26"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="12" t="s">
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="I31" s="12"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="30"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="26"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="26"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="26"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="22"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="26"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="26"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="26"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="22"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="26"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="22"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="26"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="22"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="26"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="22"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="26"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="41"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="C36:E41"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="C6:I6"/>
@@ -1281,9 +1404,14 @@
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="C36:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="97" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mpesimo 10142025 0333pm - UPDATE
</commit_message>
<xml_diff>
--- a/Portal/AttendanceCorrectionAttachments/Attendance_Correction_Template.xlsx
+++ b/Portal/AttendanceCorrectionAttachments/Attendance_Correction_Template.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APW SYSTEM\SOURCE CODE\APWPortal-WEB-UI\Portal\AttendanceCorrectionAttachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EED18C-02E2-46B8-92B7-472449EC1645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D238E278-D350-4C0A-BFFD-B1AC16A63349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8BE08107-396F-4978-B693-58822A82BF65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8BE08107-396F-4978-B693-58822A82BF65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -117,6 +117,7 @@
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -343,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -351,48 +352,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -401,58 +360,96 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AED674C-8533-4677-952F-64DCC057D066}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection sqref="A1:J41"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,68 +861,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="21"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="26"/>
+      <c r="A2" s="8"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="26"/>
+      <c r="A3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="26"/>
+      <c r="A4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="26"/>
+      <c r="A5" s="8"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="8"/>
       <c r="C6" s="28" t="s">
         <v>0</v>
       </c>
@@ -935,457 +908,351 @@
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
-      <c r="J6" s="26"/>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="26"/>
+      <c r="A7" s="8"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="29" t="s">
+      <c r="A8" s="8"/>
+      <c r="G8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="26"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="26"/>
+      <c r="A9" s="8"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="29" t="s">
+      <c r="A10" s="8"/>
+      <c r="C10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="26"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="29" t="s">
+      <c r="A11" s="8"/>
+      <c r="C11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="26"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
+      <c r="A12" s="8"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="26"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="31" t="s">
+      <c r="A13" s="8"/>
+      <c r="C13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="26"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="29" t="s">
+      <c r="A14" s="8"/>
+      <c r="C14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="26"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="29" t="s">
+      <c r="A15" s="8"/>
+      <c r="C15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="26"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="26"/>
+      <c r="A16" s="8"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="31" t="s">
+      <c r="A17" s="8"/>
+      <c r="C17" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="26"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="26"/>
+      <c r="A18" s="8"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="26"/>
+      <c r="A19" s="8"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="26"/>
+      <c r="A20" s="8"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="26"/>
+      <c r="A21" s="8"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="26"/>
+      <c r="A22" s="8"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24" t="s">
+      <c r="A23" s="8"/>
+      <c r="C23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23" t="s">
+      <c r="H23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="23"/>
-      <c r="J23" s="26"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="26"/>
+      <c r="A24" s="8"/>
+      <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="26"/>
+      <c r="A25" s="8"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="35" t="s">
+      <c r="A26" s="8"/>
+      <c r="C26" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="35" t="s">
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I26" s="35"/>
-      <c r="J26" s="26"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="10"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="26"/>
+      <c r="A27" s="8"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="24" t="s">
+      <c r="A28" s="8"/>
+      <c r="C28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23" t="s">
+      <c r="H28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I28" s="23"/>
-      <c r="J28" s="26"/>
+      <c r="J28" s="10"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="26"/>
+      <c r="A29" s="8"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="10"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="26"/>
+      <c r="A30" s="8"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="10"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="35" t="s">
+      <c r="A31" s="8"/>
+      <c r="C31" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="35" t="s">
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="I31" s="35"/>
-      <c r="J31" s="26"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="10"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="26"/>
+      <c r="A32" s="8"/>
+      <c r="J32" s="10"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="26"/>
+      <c r="A33" s="8"/>
+      <c r="J33" s="10"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="26"/>
+      <c r="A34" s="8"/>
+      <c r="J34" s="10"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="26"/>
+      <c r="A35" s="8"/>
+      <c r="J35" s="10"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="26"/>
+      <c r="A36" s="8"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="J36" s="10"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="26"/>
+      <c r="A37" s="8"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="J37" s="10"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="26"/>
+      <c r="A38" s="8"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="J38" s="10"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="26"/>
+      <c r="A39" s="8"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="J39" s="10"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="26"/>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="41"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="44"/>
+      <c r="A40" s="8"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="J40" s="10"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="19"/>
+      <c r="J41" s="10"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="19"/>
+      <c r="J42" s="10"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="20"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -1408,7 +1275,7 @@
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="H31:I31"/>
-    <mergeCell ref="C36:E41"/>
+    <mergeCell ref="C36:E43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="97" orientation="portrait" r:id="rId1"/>

</xml_diff>